<commit_message>
Main pagal ho raha hu
</commit_message>
<xml_diff>
--- a/files/samples/1_CSA.xlsx
+++ b/files/samples/1_CSA.xlsx
@@ -24,9 +24,6 @@
     <t>CLASS 1 (2017)</t>
   </si>
   <si>
-    <t>Scholar  Number</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Sharma</t>
+  </si>
+  <si>
+    <t>Roll No</t>
   </si>
 </sst>
 </file>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,7 +617,7 @@
     </row>
     <row r="3" spans="1:14" ht="21">
       <c r="A3" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -636,42 +636,42 @@
     <row r="5" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:14" ht="55.5" customHeight="1" thickBot="1">
       <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>9</v>
@@ -700,10 +700,10 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2">
-        <v>222</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
         <v>8</v>
@@ -732,10 +732,10 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2">
-        <v>333</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
         <v>7</v>

</xml_diff>